<commit_message>
Updates output variable names
</commit_message>
<xml_diff>
--- a/projects/ptool_full_factorial.xlsx
+++ b/projects/ptool_full_factorial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24930" windowHeight="12015" tabRatio="562"/>
+    <workbookView xWindow="15345" yWindow="-15" windowWidth="15390" windowHeight="13920" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="750">
   <si>
     <t>type</t>
   </si>
@@ -2202,63 +2202,6 @@
     <t>$1.71/hour</t>
   </si>
   <si>
-    <t>inject_osm_geometry_into_an_external_idf</t>
-  </si>
-  <si>
-    <t>modify_energy_management_system</t>
-  </si>
-  <si>
-    <t>ModifyEnergyManagementSystem</t>
-  </si>
-  <si>
-    <t>Standard Reports</t>
-  </si>
-  <si>
-    <t>StandardReports</t>
-  </si>
-  <si>
-    <t>../shelter_seeds/translation.osm</t>
-  </si>
-  <si>
-    <t>idf</t>
-  </si>
-  <si>
-    <t>../shelter_lib</t>
-  </si>
-  <si>
-    <t>../shelter_weather/*.epw</t>
-  </si>
-  <si>
-    <t>Directory</t>
-  </si>
-  <si>
-    <t>../../../lib/idf/AirBeam_June_v12_16.idf</t>
-  </si>
-  <si>
-    <t>mValue Floor</t>
-  </si>
-  <si>
-    <t>mValue InnerShellInsideFace</t>
-  </si>
-  <si>
-    <t>mValue InnerShellOutsideFace</t>
-  </si>
-  <si>
-    <t>mValue OuterShellInsideFace</t>
-  </si>
-  <si>
-    <t>mValue_floor</t>
-  </si>
-  <si>
-    <t>mValue_innershellinsideface</t>
-  </si>
-  <si>
-    <t>mValue_innershelloutsideface</t>
-  </si>
-  <si>
-    <t>mValue_outershellinsideface</t>
-  </si>
-  <si>
     <t>full_factorial</t>
   </si>
   <si>
@@ -2271,37 +2214,82 @@
     <t>discrete_uncertain</t>
   </si>
   <si>
-    <t>|1,2,3|</t>
-  </si>
-  <si>
-    <t>|4,5,6|</t>
-  </si>
-  <si>
-    <t>|6,7,8|</t>
-  </si>
-  <si>
-    <t>[1,2,3]</t>
-  </si>
-  <si>
-    <t>[4,5,6]</t>
-  </si>
-  <si>
-    <t>[6,7,8]</t>
-  </si>
-  <si>
-    <t>[6,7,8,9]</t>
-  </si>
-  <si>
     <t>../measures</t>
   </si>
   <si>
     <t>../../OpenStudio-Prototype-Buildings</t>
   </si>
   <si>
-    <t>Ptool Run</t>
-  </si>
-  <si>
     <t>DOE Prototype</t>
+  </si>
+  <si>
+    <t>Ptool Full Factorial</t>
+  </si>
+  <si>
+    <t>../weather/*.epw</t>
+  </si>
+  <si>
+    <t>../seeds/empty_model.osm</t>
+  </si>
+  <si>
+    <t>Create DOE Prototype Building</t>
+  </si>
+  <si>
+    <t>create_DOE_prototype_building</t>
+  </si>
+  <si>
+    <t>CreateDOEPrototypeBuilding</t>
+  </si>
+  <si>
+    <t>Building Type</t>
+  </si>
+  <si>
+    <t>building_type</t>
+  </si>
+  <si>
+    <t>SmallOffice</t>
+  </si>
+  <si>
+    <t>|SmallOffice|</t>
+  </si>
+  <si>
+    <t>Building Vintage</t>
+  </si>
+  <si>
+    <t>building_vintage</t>
+  </si>
+  <si>
+    <t>DOE Ref Pre-1980</t>
+  </si>
+  <si>
+    <t>|DOE Ref Pre-1980,DOE Ref 1980-2004,90.1-2010|</t>
+  </si>
+  <si>
+    <t>Climate Zone</t>
+  </si>
+  <si>
+    <t>climate_zone</t>
+  </si>
+  <si>
+    <t>ASHRAE 169-2006-2A</t>
+  </si>
+  <si>
+    <t>|ASHRAE 169-2006-2A,ASHRAE 169-2006-3B,ASHRAE 169-2006-4A,ASHRAE 169-2006-5A|</t>
+  </si>
+  <si>
+    <t>ASHRAE 169-2006-5A</t>
+  </si>
+  <si>
+    <t>ASHRAE 169-2006-3B</t>
+  </si>
+  <si>
+    <t>[SmallOffice]</t>
+  </si>
+  <si>
+    <t>[DOE Ref Pre-1980,DOE Ref 1980-2004,90.1-2010]</t>
+  </si>
+  <si>
+    <t>[ASHRAE 169-2006-2A,ASHRAE 169-2006-3B,ASHRAE 169-2006-4A,ASHRAE 169-2006-5A]</t>
   </si>
 </sst>
 </file>
@@ -2368,7 +2356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2423,6 +2411,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3916,7 +3910,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4007,6 +4001,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5791,10 +5786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5965,7 +5960,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>752</v>
+        <v>727</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -5976,7 +5971,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>750</v>
+        <v>724</v>
       </c>
       <c r="F14" s="33" t="s">
         <v>615</v>
@@ -5987,7 +5982,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>751</v>
+        <v>725</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -6069,7 +6064,7 @@
         <v>452</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>740</v>
+        <v>721</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -6284,7 +6279,7 @@
       <c r="E38" s="11"/>
       <c r="F38" s="13"/>
     </row>
-    <row r="39" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
@@ -6315,13 +6310,13 @@
         <v>31</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>753</v>
+        <v>726</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D42" s="41" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>449</v>
@@ -6343,20 +6338,9 @@
         <v>613</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>729</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>727</v>
-      </c>
-    </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="5">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
       <formula1>AnalysisType</formula1>
     </dataValidation>
@@ -6385,16 +6369,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -6443,14 +6427,14 @@
       <c r="R1" s="24"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -6545,247 +6529,133 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="43" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
+        <v>730</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>731</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>732</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>733</v>
+      </c>
+      <c r="E5" t="s">
+        <v>734</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" t="s">
+        <v>735</v>
+      </c>
+      <c r="J5" t="s">
+        <v>736</v>
+      </c>
+      <c r="K5" t="s">
+        <v>735</v>
+      </c>
+      <c r="L5" t="s">
+        <v>735</v>
+      </c>
+      <c r="M5" t="s">
+        <v>735</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>747</v>
+      </c>
+      <c r="R5" s="32" t="s">
         <v>723</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>724</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>724</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="43" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>720</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>267</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="32" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" s="32" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>737</v>
+      </c>
+      <c r="E6" t="s">
+        <v>738</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>739</v>
+      </c>
+      <c r="J6" t="s">
+        <v>740</v>
+      </c>
+      <c r="K6" t="s">
+        <v>739</v>
+      </c>
+      <c r="L6" t="s">
+        <v>739</v>
+      </c>
+      <c r="M6" t="s">
+        <v>739</v>
+      </c>
+      <c r="P6" s="32" t="s">
+        <v>748</v>
+      </c>
+      <c r="R6" s="32" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="43" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>721</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>721</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>722</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="32" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="32" t="s">
-        <v>731</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>735</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="32">
-        <v>1</v>
-      </c>
-      <c r="J9" s="32" t="s">
+      <c r="D7" t="s">
+        <v>741</v>
+      </c>
+      <c r="E7" t="s">
+        <v>742</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
         <v>743</v>
       </c>
-      <c r="K9" s="32">
-        <v>1</v>
-      </c>
-      <c r="L9" s="32">
-        <v>3</v>
-      </c>
-      <c r="M9" s="32">
-        <v>2</v>
-      </c>
-      <c r="N9" s="32">
-        <f>(L9-K9)/6</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P9" s="32" t="s">
+      <c r="J7" t="s">
+        <v>744</v>
+      </c>
+      <c r="K7" t="s">
+        <v>743</v>
+      </c>
+      <c r="L7" t="s">
+        <v>745</v>
+      </c>
+      <c r="M7" t="s">
         <v>746</v>
       </c>
-      <c r="R9" s="32" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" s="32" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B10" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>732</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>736</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="32">
-        <v>5</v>
-      </c>
-      <c r="J10" s="32" t="s">
-        <v>744</v>
-      </c>
-      <c r="K10" s="32">
-        <v>4</v>
-      </c>
-      <c r="L10" s="32">
-        <v>6</v>
-      </c>
-      <c r="M10" s="32">
-        <v>5</v>
-      </c>
-      <c r="N10" s="32">
-        <f>(L10-K10)/6</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P10" s="32" t="s">
-        <v>747</v>
-      </c>
-      <c r="R10" s="32" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="32" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B11" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>733</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>737</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="32">
-        <v>7</v>
-      </c>
-      <c r="J11" s="32" t="s">
-        <v>745</v>
-      </c>
-      <c r="K11" s="32">
-        <v>6</v>
-      </c>
-      <c r="L11" s="32">
-        <v>8</v>
-      </c>
-      <c r="M11" s="32">
-        <v>7</v>
-      </c>
-      <c r="N11" s="32">
-        <f>(L11-K11)/6</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P11" s="32" t="s">
+      <c r="P7" s="32" t="s">
         <v>749</v>
       </c>
-      <c r="R11" s="32" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="32" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>734</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>738</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="32">
-        <v>7</v>
-      </c>
-      <c r="J12" s="32" t="s">
-        <v>745</v>
-      </c>
-      <c r="K12" s="32">
-        <v>6</v>
-      </c>
-      <c r="L12" s="32">
-        <v>8</v>
-      </c>
-      <c r="M12" s="32">
-        <v>7</v>
-      </c>
-      <c r="N12" s="32">
-        <f>(L12-K12)/6</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P12" s="32" t="s">
-        <v>748</v>
-      </c>
-      <c r="R12" s="32" t="s">
-        <v>742</v>
-      </c>
-    </row>
+      <c r="R7" s="32" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:26" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:26" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:26" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:26" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:26" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:26" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
@@ -6812,76 +6682,72 @@
     <row r="36" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" s="33" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C40" s="32"/>
+      <c r="F40" s="33"/>
+    </row>
+    <row r="41" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C41" s="32"/>
+      <c r="F41" s="33"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="S41" s="1"/>
+    </row>
+    <row r="42" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C42" s="32"/>
+      <c r="F42" s="33"/>
+    </row>
+    <row r="43" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C43" s="32"/>
+      <c r="F43" s="33"/>
+      <c r="H43" s="1"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-    </row>
-    <row r="44" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="S43" s="1"/>
+    </row>
+    <row r="44" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A44"/>
+      <c r="B44"/>
       <c r="C44" s="32"/>
-      <c r="F44" s="33"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44" s="25"/>
+      <c r="X44" s="25"/>
+      <c r="Y44" s="25"/>
     </row>
     <row r="45" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C45" s="32"/>
       <c r="F45" s="33"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
-      <c r="S45" s="1"/>
-    </row>
-    <row r="46" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C46" s="32"/>
-      <c r="F46" s="33"/>
-    </row>
-    <row r="47" spans="1:25" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C47" s="32"/>
-      <c r="F47" s="33"/>
-      <c r="H47" s="1"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="S47" s="1"/>
-    </row>
-    <row r="48" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48" s="32"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-      <c r="N48"/>
-      <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-      <c r="S48"/>
-      <c r="T48"/>
-      <c r="U48"/>
-      <c r="V48"/>
-      <c r="W48" s="25"/>
-      <c r="X48" s="25"/>
-      <c r="Y48" s="25"/>
-    </row>
-    <row r="49" spans="3:19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C49" s="32"/>
-      <c r="F49" s="33"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="25"/>
-      <c r="S49" s="25"/>
-    </row>
-    <row r="50" spans="3:19" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C50" s="33"/>
-      <c r="I50" s="1"/>
-      <c r="K50" s="4"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="25"/>
+      <c r="S45" s="25"/>
+    </row>
+    <row r="46" spans="1:25" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C46" s="33"/>
+      <c r="I46" s="1"/>
+      <c r="K46" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -7713,16 +7579,16 @@
     <row r="42" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B42" s="32"/>
     </row>
-    <row r="43" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
     </row>
-    <row r="44" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
     </row>
-    <row r="45" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
     </row>
-    <row r="46" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
@@ -8823,7 +8689,7 @@
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
       <c r="B42" s="17" t="s">
         <v>21</v>
@@ -8844,7 +8710,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="17" t="s">
         <v>21</v>
@@ -8867,7 +8733,7 @@
       </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="17" t="s">
         <v>21</v>
@@ -8890,7 +8756,7 @@
       </c>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>21</v>
@@ -16328,7 +16194,7 @@
         <v>551</v>
       </c>
       <c r="F20" t="s">
-        <v>740</v>
+        <v>721</v>
       </c>
       <c r="I20" t="s">
         <v>559</v>
@@ -16351,13 +16217,13 @@
         <v>551</v>
       </c>
       <c r="F21" t="s">
-        <v>741</v>
+        <v>722</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>739</v>
+        <v>720</v>
       </c>
       <c r="H21" t="s">
-        <v>739</v>
+        <v>720</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>540</v>
@@ -16389,7 +16255,7 @@
     </row>
     <row r="22" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>740</v>
+        <v>721</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Updates full factorial of base buildings and preflight check run
</commit_message>
<xml_diff>
--- a/projects/ptool_full_factorial.xlsx
+++ b/projects/ptool_full_factorial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="-15" windowWidth="15390" windowHeight="13920" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="15345" yWindow="-15" windowWidth="9855" windowHeight="12390" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="748">
   <si>
     <t>type</t>
   </si>
@@ -2250,9 +2250,6 @@
     <t>SmallOffice</t>
   </si>
   <si>
-    <t>|SmallOffice|</t>
-  </si>
-  <si>
     <t>Building Vintage</t>
   </si>
   <si>
@@ -2277,19 +2274,16 @@
     <t>|ASHRAE 169-2006-2A,ASHRAE 169-2006-3B,ASHRAE 169-2006-4A,ASHRAE 169-2006-5A|</t>
   </si>
   <si>
-    <t>ASHRAE 169-2006-5A</t>
-  </si>
-  <si>
-    <t>ASHRAE 169-2006-3B</t>
-  </si>
-  <si>
-    <t>[SmallOffice]</t>
-  </si>
-  <si>
     <t>[DOE Ref Pre-1980,DOE Ref 1980-2004,90.1-2010]</t>
   </si>
   <si>
     <t>[ASHRAE 169-2006-2A,ASHRAE 169-2006-3B,ASHRAE 169-2006-4A,ASHRAE 169-2006-5A]</t>
+  </si>
+  <si>
+    <t>|SmallOffice,SecondarySchool|</t>
+  </si>
+  <si>
+    <t>[SmallOffice,SecondarySchool]</t>
   </si>
 </sst>
 </file>
@@ -6372,7 +6366,7 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6548,7 +6542,7 @@
     </row>
     <row r="5" spans="1:26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>733</v>
@@ -6563,12 +6557,12 @@
         <v>735</v>
       </c>
       <c r="J5" t="s">
-        <v>736</v>
+        <v>746</v>
       </c>
       <c r="K5" t="s">
         <v>735</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="32" t="s">
         <v>735</v>
       </c>
       <c r="M5" t="s">
@@ -6586,31 +6580,31 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>736</v>
+      </c>
+      <c r="E6" t="s">
         <v>737</v>
-      </c>
-      <c r="E6" t="s">
-        <v>738</v>
       </c>
       <c r="G6" t="s">
         <v>61</v>
       </c>
       <c r="I6" t="s">
+        <v>738</v>
+      </c>
+      <c r="J6" t="s">
         <v>739</v>
       </c>
-      <c r="J6" t="s">
-        <v>740</v>
-      </c>
       <c r="K6" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="L6" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="M6" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="P6" s="32" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="R6" s="32" t="s">
         <v>723</v>
@@ -6621,31 +6615,31 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
+        <v>740</v>
+      </c>
+      <c r="E7" t="s">
         <v>741</v>
-      </c>
-      <c r="E7" t="s">
-        <v>742</v>
       </c>
       <c r="G7" t="s">
         <v>61</v>
       </c>
       <c r="I7" t="s">
+        <v>742</v>
+      </c>
+      <c r="J7" t="s">
         <v>743</v>
       </c>
-      <c r="J7" t="s">
-        <v>744</v>
-      </c>
       <c r="K7" t="s">
-        <v>743</v>
-      </c>
-      <c r="L7" t="s">
+        <v>742</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>742</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>742</v>
+      </c>
+      <c r="P7" s="32" t="s">
         <v>745</v>
-      </c>
-      <c r="M7" t="s">
-        <v>746</v>
-      </c>
-      <c r="P7" s="32" t="s">
-        <v>749</v>
       </c>
       <c r="R7" s="32" t="s">
         <v>723</v>

</xml_diff>